<commit_message>
dialog fyrir booked trip
</commit_message>
<xml_diff>
--- a/Progress_Tracking_sheet_9d.xlsx
+++ b/Progress_Tracking_sheet_9d.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leifu\Documents\Verkefni\Þróun Hugbúnaðar git\hbv401G-9d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnar\Desktop\Skóldót\4. Misseri\Þróun hugbúnaðar\hop-9d\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C3175E-40C1-4A76-992D-FB647EA4C8FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>User Story ID</t>
   </si>
@@ -117,6 +118,12 @@
   </si>
   <si>
     <t>[9D -Arnar Pétursson  arp25@hi.is Freyr Saputra Daníelsson fsd1@hi.is Leifur Daníel Sigurðarson lsd2@hi.is ]</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -195,7 +202,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -473,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,6 +576,9 @@
       <c r="F4" s="3">
         <v>2</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
@@ -558,6 +599,9 @@
       <c r="F5" s="3">
         <v>1</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
@@ -578,6 +622,9 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -595,6 +642,9 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
@@ -612,6 +662,9 @@
       <c r="E8" s="3">
         <v>10</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
@@ -629,6 +682,9 @@
       <c r="E9" s="3">
         <v>3</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
@@ -646,6 +702,9 @@
       <c r="E10" s="3">
         <v>13</v>
       </c>
+      <c r="G10" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
@@ -663,6 +722,9 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
+      <c r="G11" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
@@ -680,6 +742,9 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
@@ -697,6 +762,9 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
+      <c r="G13" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
@@ -714,6 +782,9 @@
       <c r="E14" s="3">
         <v>2</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
@@ -731,6 +802,9 @@
       <c r="E15" s="3">
         <v>2</v>
       </c>
+      <c r="G15" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
@@ -748,8 +822,11 @@
       <c r="E16" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>3</v>
       </c>
@@ -765,8 +842,11 @@
       <c r="E17" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -782,8 +862,11 @@
       <c r="E18" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>4</v>
       </c>
@@ -799,8 +882,11 @@
       <c r="E19" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>4</v>
       </c>
@@ -816,8 +902,14 @@
       <c r="E20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="3">
+        <v>4</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>4</v>
       </c>
@@ -833,8 +925,11 @@
       <c r="E21" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G21" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>5</v>
       </c>
@@ -850,8 +945,11 @@
       <c r="E22" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G22" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -867,8 +965,11 @@
       <c r="E23" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G23" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
@@ -877,6 +978,14 @@
   <sortState ref="A4:G23">
     <sortCondition ref="D4"/>
   </sortState>
+  <conditionalFormatting sqref="G4:G23">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
klasadiagram og excel skjal
</commit_message>
<xml_diff>
--- a/Progress_Tracking_sheet_9d.xlsx
+++ b/Progress_Tracking_sheet_9d.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnar\Desktop\Skóldót\4. Misseri\Þróun hugbúnaðar\hop-9d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C3175E-40C1-4A76-992D-FB647EA4C8FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE7ECED-4539-4E10-B447-349609370570}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,30 +54,18 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>As a marketing manager, I want to reply to reviews in public or private, in order to address any mentioned concerns.</t>
-  </si>
-  <si>
     <t>As a website visitor it is crucial for me that the website is available in english.</t>
   </si>
   <si>
     <t xml:space="preserve">As a customer, I want to endorse reviews that i agree with, to make the review more reliable. </t>
   </si>
   <si>
-    <t>As a traveler, I would like to see tours that are on special offer, to be able to find something that i might like with better pricing.</t>
-  </si>
-  <si>
     <t>As a tourist, I want to submit a review for a day tour I've been on, to let others know what my experience was and what to expect</t>
   </si>
   <si>
     <t>As a webmaster, I want to be able to verify reviews before they appear on the website, to make sure it isn't spam</t>
   </si>
   <si>
-    <t>As a website visitor, I want to see what tours are popular, so I don't have to spend time searching for good tours</t>
-  </si>
-  <si>
-    <t>As a website visitor, I want to see photos from day tours, so I know what to expect</t>
-  </si>
-  <si>
     <t>As a website visitor, I would like to see the duration of each tour so I can plan my day efficiently</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
     <t>As a website visitor, I would like to be able to book the tours I am interested in, to secure my place in the trip.</t>
   </si>
   <si>
-    <t>As a website visitor, I would like to receive a confirmation email for the trips I have booked, to ensure my booking took place.</t>
-  </si>
-  <si>
     <t xml:space="preserve">As a tourist, I would like to receive a reminder email the day before, so I don´t forget my trip. </t>
   </si>
   <si>
@@ -124,6 +109,21 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>As a website visitor, I would like to receive a confirmation that I have booked, to ensure my booking took place.</t>
+  </si>
+  <si>
+    <t>As a tourist, I would like to be able to search for tours that do pickup, so I can plan my day efficiently.</t>
+  </si>
+  <si>
+    <t>As a marketing manager, I would like to be able to make a new trip, so it can be viewed on the site</t>
+  </si>
+  <si>
+    <t>As a traveler, I would like to search for tours depending on their difficulty, so I can filter out tours I am not fit enough for</t>
+  </si>
+  <si>
+    <t>As a marketing manager, I want to be able to accept all pending reviews, to save time when I know reviews are not spam</t>
   </si>
 </sst>
 </file>
@@ -202,17 +202,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -511,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>7</v>
@@ -565,7 +555,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -574,10 +564,10 @@
         <v>6</v>
       </c>
       <c r="F4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -588,7 +578,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -600,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -611,7 +601,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -623,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -634,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -642,8 +632,11 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -654,7 +647,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>40</v>
@@ -662,8 +655,11 @@
       <c r="E8" s="3">
         <v>10</v>
       </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
       <c r="G8" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -674,7 +670,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -682,8 +678,11 @@
       <c r="E9" s="3">
         <v>3</v>
       </c>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
       <c r="G9" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -694,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -703,7 +702,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -714,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -722,8 +721,11 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
       <c r="G11" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -734,7 +736,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -742,8 +744,11 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
       <c r="G12" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -754,7 +759,7 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -762,8 +767,11 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
       <c r="G13" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -774,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>70</v>
@@ -782,8 +790,11 @@
       <c r="E14" s="3">
         <v>2</v>
       </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
       <c r="G14" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -794,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>80</v>
@@ -802,8 +813,11 @@
       <c r="E15" s="3">
         <v>2</v>
       </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
       <c r="G15" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -814,16 +828,19 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>90</v>
       </c>
       <c r="E16" s="3">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -834,16 +851,19 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>100</v>
       </c>
       <c r="E17" s="3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -854,7 +874,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>110</v>
@@ -863,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -874,7 +894,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D19">
         <v>110</v>
@@ -883,7 +903,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -894,7 +914,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>120</v>
@@ -906,7 +926,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -917,16 +937,19 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D21">
         <v>130</v>
       </c>
       <c r="E21" s="3">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -937,7 +960,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D22">
         <v>140</v>
@@ -946,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -957,7 +980,7 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D23">
         <v>140</v>
@@ -966,12 +989,12 @@
         <v>3</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E25" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -979,10 +1002,10 @@
     <sortCondition ref="D4"/>
   </sortState>
   <conditionalFormatting sqref="G4:G23">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>